<commit_message>
the screen is not cleared and not blinked
</commit_message>
<xml_diff>
--- a/ADC_time-F3.xlsx
+++ b/ADC_time-F3.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Java processing" sheetId="2" r:id="rId2"/>
-    <sheet name="Triangle" sheetId="3" r:id="rId3"/>
-    <sheet name="TIM Generator" sheetId="4" r:id="rId4"/>
+    <sheet name="ADC" sheetId="1" r:id="rId1"/>
+    <sheet name="TIM Generator" sheetId="4" r:id="rId2"/>
+    <sheet name="Java processing" sheetId="2" r:id="rId3"/>
+    <sheet name="Triangle" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -554,7 +554,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$6:$L$6</c:f>
+              <c:f>ADC!$E$6:$L$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -587,7 +587,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$7:$L$7</c:f>
+              <c:f>ADC!$E$7:$L$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -654,7 +654,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$6:$L$6</c:f>
+              <c:f>ADC!$E$6:$L$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -687,7 +687,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$8:$L$8</c:f>
+              <c:f>ADC!$E$8:$L$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -754,7 +754,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$6:$L$6</c:f>
+              <c:f>ADC!$E$6:$L$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -787,7 +787,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$9:$L$9</c:f>
+              <c:f>ADC!$E$9:$L$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1890,7 +1890,7 @@
   <dimension ref="B2:L68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3672,6 +3672,170 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>72000000</v>
+      </c>
+      <c r="C3">
+        <f>B3*2</f>
+        <v>144000000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>71</v>
+      </c>
+      <c r="C6">
+        <f>$C$3/(B6+1)</f>
+        <v>2000000</v>
+      </c>
+      <c r="D6">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <f>C6/(D6+1)</f>
+        <v>100000</v>
+      </c>
+      <c r="G6">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>71</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:C11" si="0">$C$3/(B7+1)</f>
+        <v>2000000</v>
+      </c>
+      <c r="D7">
+        <v>24</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:E11" si="1">C7/(D7+1)</f>
+        <v>80000</v>
+      </c>
+      <c r="G7">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>49</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>2880000</v>
+      </c>
+      <c r="D8">
+        <v>47</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>60000</v>
+      </c>
+      <c r="G8">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>71</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>2000000</v>
+      </c>
+      <c r="D9">
+        <v>49</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+      <c r="G9">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>71</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2000000</v>
+      </c>
+      <c r="D10">
+        <v>99</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>20000</v>
+      </c>
+      <c r="G10">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>71</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>2000000</v>
+      </c>
+      <c r="D11">
+        <v>199</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="G11">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:B70"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
@@ -3975,7 +4139,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B27"/>
   <sheetViews>
@@ -4089,168 +4253,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>72000000</v>
-      </c>
-      <c r="C3">
-        <f>B3*2</f>
-        <v>144000000</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>71</v>
-      </c>
-      <c r="C6">
-        <f>$C$3/(B6+1)</f>
-        <v>2000000</v>
-      </c>
-      <c r="D6">
-        <v>19</v>
-      </c>
-      <c r="E6">
-        <f>C6/(D6+1)</f>
-        <v>100000</v>
-      </c>
-      <c r="G6">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>71</v>
-      </c>
-      <c r="C7">
-        <f t="shared" ref="C7:C11" si="0">$C$3/(B7+1)</f>
-        <v>2000000</v>
-      </c>
-      <c r="D7">
-        <v>24</v>
-      </c>
-      <c r="E7">
-        <f t="shared" ref="E7:E11" si="1">C7/(D7+1)</f>
-        <v>80000</v>
-      </c>
-      <c r="G7">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>49</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>2880000</v>
-      </c>
-      <c r="D8">
-        <v>47</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="1"/>
-        <v>60000</v>
-      </c>
-      <c r="G8">
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>71</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>2000000</v>
-      </c>
-      <c r="D9">
-        <v>49</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
-        <v>40000</v>
-      </c>
-      <c r="G9">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>71</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>2000000</v>
-      </c>
-      <c r="D10">
-        <v>99</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="1"/>
-        <v>20000</v>
-      </c>
-      <c r="G10">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>71</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>2000000</v>
-      </c>
-      <c r="D11">
-        <v>199</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
-        <v>10000</v>
-      </c>
-      <c r="G11">
-        <v>10000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>